<commit_message>
Convert files to .xlsx
Github doesnt sense csv files
</commit_message>
<xml_diff>
--- a/CoilDesign/AnalysisResults_Block/FerriteBlock.xlsx
+++ b/CoilDesign/AnalysisResults_Block/FerriteBlock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Documents\GitHub\2020-srw-rc-car\CoilDesign\AnalysisResults_Block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A17FB1-0F5C-4ED8-9CA1-4F9FDB572B8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F5EC1-F433-44A1-AD0E-EA07A8D2EAC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9968,8 +9968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B8707C-0ADA-43C9-8138-8806A8046C6B}">
   <dimension ref="B1:AA290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10031,6 +10031,11 @@
       <c r="K2">
         <f>2*PI()*K1</f>
         <v>942477.79607693793</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added data from more sweeps
Re ran some sweeps due to conflicting data; data changes each time we run the sweep
</commit_message>
<xml_diff>
--- a/CoilDesign/AnalysisResults_Block/FerriteBlock.xlsx
+++ b/CoilDesign/AnalysisResults_Block/FerriteBlock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Documents\GitHub\2020-srw-rc-car\CoilDesign\AnalysisResults_Block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F5EC1-F433-44A1-AD0E-EA07A8D2EAC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B07409-325D-4601-B95D-32641FBE083A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ydisp" sheetId="6" r:id="rId1"/>
@@ -3793,7 +3793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5C03A5-8D53-4612-89BE-2250A06B9300}">
   <dimension ref="B1:AA294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -9968,7 +9968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B8707C-0ADA-43C9-8138-8806A8046C6B}">
   <dimension ref="B1:AA290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>